<commit_message>
Update Technical Reports-Research Proposals-Projects-Thesis-Capstone Projects-Dissertations-Version-3.xlsx
</commit_message>
<xml_diff>
--- a/Technical Reports-Research Proposals-Projects-Thesis-Capstone Projects-Dissertations-Version-3.xlsx
+++ b/Technical Reports-Research Proposals-Projects-Thesis-Capstone Projects-Dissertations-Version-3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a2b7f844a7ade77c/Documents/GitHub/ACADEMIC-SCHOLARLY-AND-PRACTICAL-APPLIED-WORKS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{B49B52A3-B6CA-4DEF-828A-6BBF2E9D54A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AA6B7A1-28EF-4A13-97CB-1C3EE6910DC4}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{B49B52A3-B6CA-4DEF-828A-6BBF2E9D54A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A0332A3-619C-48C7-8782-B3772FF5E229}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2412,7 +2412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2429,9 +2429,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2447,6 +2444,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2748,8 +2749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A371" workbookViewId="0">
-      <selection activeCell="A363" sqref="A363"/>
+    <sheetView tabSelected="1" topLeftCell="A363" workbookViewId="0">
+      <selection activeCell="B237" sqref="B237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -5890,11 +5891,11 @@
         <v>149</v>
       </c>
     </row>
-    <row r="191" spans="1:5" ht="96.6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>152.19999999999999</v>
       </c>
-      <c r="B191" s="6" t="s">
+      <c r="B191" s="5" t="s">
         <v>382</v>
       </c>
       <c r="C191" s="2" t="s">
@@ -6649,11 +6650,11 @@
         <v>149</v>
       </c>
     </row>
-    <row r="236" spans="1:5" ht="96.6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>165.1</v>
       </c>
-      <c r="B236" s="6" t="s">
+      <c r="B236" s="5" t="s">
         <v>470</v>
       </c>
       <c r="C236" s="1" t="s">
@@ -6666,11 +6667,11 @@
         <v>149</v>
       </c>
     </row>
-    <row r="237" spans="1:5" ht="96.6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>165.2</v>
       </c>
-      <c r="B237" s="6" t="s">
+      <c r="B237" s="5" t="s">
         <v>471</v>
       </c>
       <c r="C237" s="1" t="s">
@@ -8776,6 +8777,71 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <NotebookType xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <FolderType xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <Teachers xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <DefaultSectionNames xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <Owner xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Is_Collaboration_Space_Locked xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <TaxCatchAll xmlns="d7bec7bf-3da8-4078-8aa6-220bab9f77bc" xsi:nil="true"/>
+    <CultureName xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <Distribution_Groups xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <AppVersion xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <Invited_Students xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <Student_Groups xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Math_Settings xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <Templates xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <TeamsChannelId xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <Invited_Teachers xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Students xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Self_Registration_Enabled xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+    <LMS_Mappings xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010039D1DEEADAC1A5458EF0D48482917E3D" ma:contentTypeVersion="36" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b7aea47dc6ae66664ea90708d5997129">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xmlns:ns3="d7bec7bf-3da8-4078-8aa6-220bab9f77bc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="98593b28f1f0b1cf1ed3518b24bbb869" ns2:_="" ns3:_="">
     <xsd:import namespace="64465c1d-2775-432b-8ccf-8b9a5bbd2975"/>
@@ -9206,72 +9272,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC8EB3D1-86FA-41D2-9F48-D030848D8DA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="64465c1d-2775-432b-8ccf-8b9a5bbd2975"/>
+    <ds:schemaRef ds:uri="d7bec7bf-3da8-4078-8aa6-220bab9f77bc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <NotebookType xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <FolderType xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <Teachers xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <DefaultSectionNames xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <Owner xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Is_Collaboration_Space_Locked xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <TaxCatchAll xmlns="d7bec7bf-3da8-4078-8aa6-220bab9f77bc" xsi:nil="true"/>
-    <CultureName xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <Distribution_Groups xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <AppVersion xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <Invited_Students xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <Student_Groups xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Math_Settings xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <Templates xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <TeamsChannelId xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <Invited_Teachers xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Students xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Self_Registration_Enabled xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-    <LMS_Mappings xmlns="64465c1d-2775-432b-8ccf-8b9a5bbd2975" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFE1C7E4-455D-434D-B571-2B64DF7AE606}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3E60AE-CFEB-40B7-B274-53261BB6A31F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9288,23 +9308,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFE1C7E4-455D-434D-B571-2B64DF7AE606}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC8EB3D1-86FA-41D2-9F48-D030848D8DA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="64465c1d-2775-432b-8ccf-8b9a5bbd2975"/>
-    <ds:schemaRef ds:uri="d7bec7bf-3da8-4078-8aa6-220bab9f77bc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>